<commit_message>
Lots of new output files
</commit_message>
<xml_diff>
--- a/manuscript/intactness_results.xlsx
+++ b/manuscript/intactness_results.xlsx
@@ -3,16 +3,17 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20359"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D3F8606-53D7-4971-BA95-6B08957FE4D1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8301EFD-66C4-40AB-92F9-E8D857F31B98}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="datasets" sheetId="1" r:id="rId1"/>
-    <sheet name="agreement" sheetId="10" r:id="rId2"/>
-    <sheet name="pros &amp; cons" sheetId="7" r:id="rId3"/>
-    <sheet name="applications" sheetId="11" r:id="rId4"/>
-    <sheet name="case studies" sheetId="12" r:id="rId5"/>
+    <sheet name="agreement new" sheetId="13" r:id="rId2"/>
+    <sheet name="agreement" sheetId="10" r:id="rId3"/>
+    <sheet name="pros &amp; cons" sheetId="7" r:id="rId4"/>
+    <sheet name="applications" sheetId="11" r:id="rId5"/>
+    <sheet name="case studies" sheetId="12" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -82,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="204">
   <si>
     <t>Map</t>
   </si>
@@ -1152,6 +1153,30 @@
   <si>
     <t>BEAD2010, BEAD2015</t>
   </si>
+  <si>
+    <t>map1</t>
+  </si>
+  <si>
+    <t>map1_intact</t>
+  </si>
+  <si>
+    <t>map1_unique</t>
+  </si>
+  <si>
+    <t>map2</t>
+  </si>
+  <si>
+    <t>map2_intact</t>
+  </si>
+  <si>
+    <t>map2_unique</t>
+  </si>
+  <si>
+    <t>overlap_km2</t>
+  </si>
+  <si>
+    <t>overlap_pct</t>
+  </si>
 </sst>
 </file>
 
@@ -1160,9 +1185,16 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1443,121 +1475,132 @@
   </cellStyleXfs>
   <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="18" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="19" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="18" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="19" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -2305,11 +2348,1475 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76939AA6-8109-4641-AF7E-FEBDADDB1A11}">
+  <dimension ref="A1:N29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D1" t="s">
+        <v>199</v>
+      </c>
+      <c r="E1" t="s">
+        <v>200</v>
+      </c>
+      <c r="F1" t="s">
+        <v>201</v>
+      </c>
+      <c r="G1" t="s">
+        <v>202</v>
+      </c>
+      <c r="H1" t="s">
+        <v>203</v>
+      </c>
+      <c r="I1" t="s">
+        <v>158</v>
+      </c>
+      <c r="J1" t="s">
+        <v>153</v>
+      </c>
+      <c r="K1" t="s">
+        <v>154</v>
+      </c>
+      <c r="L1" t="s">
+        <v>157</v>
+      </c>
+      <c r="M1" t="s">
+        <v>156</v>
+      </c>
+      <c r="N1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B2">
+        <v>3798352.5630000001</v>
+      </c>
+      <c r="C2">
+        <v>14.7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E2">
+        <v>3294591.8130000001</v>
+      </c>
+      <c r="F2">
+        <v>1.6</v>
+      </c>
+      <c r="G2">
+        <v>3232684.375</v>
+      </c>
+      <c r="H2">
+        <v>83.7</v>
+      </c>
+      <c r="I2">
+        <f>COUNTIF($A2:$D2,I$1)</f>
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <f>COUNTIF($A2:$D2,J$1)</f>
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <f>COUNTIF($A2:$D2,K$1)</f>
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <f>COUNTIF($A2:$D2,L$1)</f>
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <f>COUNTIF($A2:$D2,M$1)</f>
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <f>COUNTIF($A2:$D2,N$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B3">
+        <v>3294591.8130000001</v>
+      </c>
+      <c r="C3">
+        <v>20.5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>157</v>
+      </c>
+      <c r="E3">
+        <v>2652405.9380000001</v>
+      </c>
+      <c r="F3">
+        <v>1.3</v>
+      </c>
+      <c r="G3">
+        <v>2608740.75</v>
+      </c>
+      <c r="H3">
+        <v>78.099999999999994</v>
+      </c>
+      <c r="I3">
+        <f>COUNTIF($A3:$D3,I$1)</f>
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <f>COUNTIF($A3:$D3,J$1)</f>
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <f>COUNTIF($A3:$D3,K$1)</f>
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <f>COUNTIF($A3:$D3,L$1)</f>
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <f>COUNTIF($A3:$D3,M$1)</f>
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <f>COUNTIF($A3:$D3,N$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>153</v>
+      </c>
+      <c r="B4">
+        <v>3798352.5630000001</v>
+      </c>
+      <c r="C4">
+        <v>7.5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>152</v>
+      </c>
+      <c r="E4">
+        <v>4143004.3130000001</v>
+      </c>
+      <c r="F4">
+        <v>15.2</v>
+      </c>
+      <c r="G4">
+        <v>3463239.25</v>
+      </c>
+      <c r="H4">
+        <v>77.3</v>
+      </c>
+      <c r="I4">
+        <f>COUNTIF($A4:$D4,I$1)</f>
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <f>COUNTIF($A4:$D4,J$1)</f>
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <f>COUNTIF($A4:$D4,K$1)</f>
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <f>COUNTIF($A4:$D4,L$1)</f>
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <f>COUNTIF($A4:$D4,M$1)</f>
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <f>COUNTIF($A4:$D4,N$1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>152</v>
+      </c>
+      <c r="B5">
+        <v>4143004.3130000001</v>
+      </c>
+      <c r="C5">
+        <v>18.399999999999999</v>
+      </c>
+      <c r="D5" t="s">
+        <v>156</v>
+      </c>
+      <c r="E5">
+        <v>3618249.5</v>
+      </c>
+      <c r="F5">
+        <v>6.6</v>
+      </c>
+      <c r="G5">
+        <v>3326867.3130000001</v>
+      </c>
+      <c r="H5">
+        <v>75</v>
+      </c>
+      <c r="I5">
+        <f>COUNTIF($A5:$D5,I$1)</f>
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <f>COUNTIF($A5:$D5,J$1)</f>
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <f>COUNTIF($A5:$D5,K$1)</f>
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <f>COUNTIF($A5:$D5,L$1)</f>
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <f>COUNTIF($A5:$D5,M$1)</f>
+        <v>1</v>
+      </c>
+      <c r="N5">
+        <f>COUNTIF($A5:$D5,N$1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>153</v>
+      </c>
+      <c r="B6">
+        <v>3798352.5630000001</v>
+      </c>
+      <c r="C6">
+        <v>15.7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>156</v>
+      </c>
+      <c r="E6">
+        <v>3618249.5</v>
+      </c>
+      <c r="F6">
+        <v>11.5</v>
+      </c>
+      <c r="G6">
+        <v>3123836.5</v>
+      </c>
+      <c r="H6">
+        <v>72.8</v>
+      </c>
+      <c r="I6">
+        <f>COUNTIF($A6:$D6,I$1)</f>
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <f>COUNTIF($A6:$D6,J$1)</f>
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <f>COUNTIF($A6:$D6,K$1)</f>
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <f>COUNTIF($A6:$D6,L$1)</f>
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <f>COUNTIF($A6:$D6,M$1)</f>
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <f>COUNTIF($A6:$D6,N$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>154</v>
+      </c>
+      <c r="B7">
+        <v>3294591.8130000001</v>
+      </c>
+      <c r="C7">
+        <v>4.2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>152</v>
+      </c>
+      <c r="E7">
+        <v>4143004.3130000001</v>
+      </c>
+      <c r="F7">
+        <v>23.9</v>
+      </c>
+      <c r="G7">
+        <v>3110954.625</v>
+      </c>
+      <c r="H7">
+        <v>71.900000000000006</v>
+      </c>
+      <c r="I7">
+        <f>COUNTIF($A7:$D7,I$1)</f>
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <f>COUNTIF($A7:$D7,J$1)</f>
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <f>COUNTIF($A7:$D7,K$1)</f>
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <f>COUNTIF($A7:$D7,L$1)</f>
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <f>COUNTIF($A7:$D7,M$1)</f>
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <f>COUNTIF($A7:$D7,N$1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>154</v>
+      </c>
+      <c r="B8">
+        <v>3294591.8130000001</v>
+      </c>
+      <c r="C8">
+        <v>17.8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>155</v>
+      </c>
+      <c r="E8">
+        <v>3041886.625</v>
+      </c>
+      <c r="F8">
+        <v>11</v>
+      </c>
+      <c r="G8">
+        <v>2636402.25</v>
+      </c>
+      <c r="H8">
+        <v>71.3</v>
+      </c>
+      <c r="I8">
+        <f>COUNTIF($A8:$D8,I$1)</f>
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <f>COUNTIF($A8:$D8,J$1)</f>
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <f>COUNTIF($A8:$D8,K$1)</f>
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <f>COUNTIF($A8:$D8,L$1)</f>
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <f>COUNTIF($A8:$D8,M$1)</f>
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <f>COUNTIF($A8:$D8,N$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>154</v>
+      </c>
+      <c r="B9">
+        <v>3294591.8130000001</v>
+      </c>
+      <c r="C9">
+        <v>10.9</v>
+      </c>
+      <c r="D9" t="s">
+        <v>156</v>
+      </c>
+      <c r="E9">
+        <v>3618249.5</v>
+      </c>
+      <c r="F9">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="G9">
+        <v>2852762.5630000001</v>
+      </c>
+      <c r="H9">
+        <v>70.3</v>
+      </c>
+      <c r="I9">
+        <f>COUNTIF($A9:$D9,I$1)</f>
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <f>COUNTIF($A9:$D9,J$1)</f>
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <f>COUNTIF($A9:$D9,K$1)</f>
+        <v>1</v>
+      </c>
+      <c r="L9">
+        <f>COUNTIF($A9:$D9,L$1)</f>
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <f>COUNTIF($A9:$D9,M$1)</f>
+        <v>1</v>
+      </c>
+      <c r="N9">
+        <f>COUNTIF($A9:$D9,N$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>158</v>
+      </c>
+      <c r="B10">
+        <v>3196063.625</v>
+      </c>
+      <c r="C10">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="D10" t="s">
+        <v>152</v>
+      </c>
+      <c r="E10">
+        <v>4143004.3130000001</v>
+      </c>
+      <c r="F10">
+        <v>26</v>
+      </c>
+      <c r="G10">
+        <v>3019862.5630000001</v>
+      </c>
+      <c r="H10">
+        <v>69.900000000000006</v>
+      </c>
+      <c r="I10">
+        <f>COUNTIF($A10:$D10,I$1)</f>
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <f>COUNTIF($A10:$D10,J$1)</f>
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <f>COUNTIF($A10:$D10,K$1)</f>
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <f>COUNTIF($A10:$D10,L$1)</f>
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <f>COUNTIF($A10:$D10,M$1)</f>
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <f>COUNTIF($A10:$D10,N$1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>153</v>
+      </c>
+      <c r="B11">
+        <v>3798352.5630000001</v>
+      </c>
+      <c r="C11">
+        <v>30.9</v>
+      </c>
+      <c r="D11" t="s">
+        <v>157</v>
+      </c>
+      <c r="E11">
+        <v>2652405.9380000001</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>2612882.1880000001</v>
+      </c>
+      <c r="H11">
+        <v>68.099999999999994</v>
+      </c>
+      <c r="I11">
+        <f>COUNTIF($A11:$D11,I$1)</f>
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <f>COUNTIF($A11:$D11,J$1)</f>
+        <v>1</v>
+      </c>
+      <c r="K11">
+        <f>COUNTIF($A11:$D11,K$1)</f>
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <f>COUNTIF($A11:$D11,L$1)</f>
+        <v>1</v>
+      </c>
+      <c r="M11">
+        <f>COUNTIF($A11:$D11,M$1)</f>
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <f>COUNTIF($A11:$D11,N$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>154</v>
+      </c>
+      <c r="B12">
+        <v>3294591.8130000001</v>
+      </c>
+      <c r="C12">
+        <v>17.3</v>
+      </c>
+      <c r="D12" t="s">
+        <v>158</v>
+      </c>
+      <c r="E12">
+        <v>3196063.625</v>
+      </c>
+      <c r="F12">
+        <v>14.8</v>
+      </c>
+      <c r="G12">
+        <v>2624449.875</v>
+      </c>
+      <c r="H12">
+        <v>67.900000000000006</v>
+      </c>
+      <c r="I12">
+        <f>COUNTIF($A12:$D12,I$1)</f>
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <f>COUNTIF($A12:$D12,J$1)</f>
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <f>COUNTIF($A12:$D12,K$1)</f>
+        <v>1</v>
+      </c>
+      <c r="L12">
+        <f>COUNTIF($A12:$D12,L$1)</f>
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <f>COUNTIF($A12:$D12,M$1)</f>
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <f>COUNTIF($A12:$D12,N$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>153</v>
+      </c>
+      <c r="B13">
+        <v>3798352.5630000001</v>
+      </c>
+      <c r="C13">
+        <v>23.7</v>
+      </c>
+      <c r="D13" t="s">
+        <v>158</v>
+      </c>
+      <c r="E13">
+        <v>3196063.625</v>
+      </c>
+      <c r="F13">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="G13">
+        <v>2804445.4380000001</v>
+      </c>
+      <c r="H13">
+        <v>66.900000000000006</v>
+      </c>
+      <c r="I13">
+        <f>COUNTIF($A13:$D13,I$1)</f>
+        <v>1</v>
+      </c>
+      <c r="J13">
+        <f>COUNTIF($A13:$D13,J$1)</f>
+        <v>1</v>
+      </c>
+      <c r="K13">
+        <f>COUNTIF($A13:$D13,K$1)</f>
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <f>COUNTIF($A13:$D13,L$1)</f>
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <f>COUNTIF($A13:$D13,M$1)</f>
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <f>COUNTIF($A13:$D13,N$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>153</v>
+      </c>
+      <c r="B14">
+        <v>3798352.5630000001</v>
+      </c>
+      <c r="C14">
+        <v>25.8</v>
+      </c>
+      <c r="D14" t="s">
+        <v>155</v>
+      </c>
+      <c r="E14">
+        <v>3041886.625</v>
+      </c>
+      <c r="F14">
+        <v>7.4</v>
+      </c>
+      <c r="G14">
+        <v>2738034.25</v>
+      </c>
+      <c r="H14">
+        <v>66.7</v>
+      </c>
+      <c r="I14">
+        <f>COUNTIF($A14:$D14,I$1)</f>
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <f>COUNTIF($A14:$D14,J$1)</f>
+        <v>1</v>
+      </c>
+      <c r="K14">
+        <f>COUNTIF($A14:$D14,K$1)</f>
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <f>COUNTIF($A14:$D14,L$1)</f>
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <f>COUNTIF($A14:$D14,M$1)</f>
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <f>COUNTIF($A14:$D14,N$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>152</v>
+      </c>
+      <c r="B15">
+        <v>4143004.3130000001</v>
+      </c>
+      <c r="C15">
+        <v>29.5</v>
+      </c>
+      <c r="D15" t="s">
+        <v>155</v>
+      </c>
+      <c r="E15">
+        <v>3041886.625</v>
+      </c>
+      <c r="F15">
+        <v>3.9</v>
+      </c>
+      <c r="G15">
+        <v>2872641.5</v>
+      </c>
+      <c r="H15">
+        <v>66.599999999999994</v>
+      </c>
+      <c r="I15">
+        <f>COUNTIF($A15:$D15,I$1)</f>
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <f>COUNTIF($A15:$D15,J$1)</f>
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <f>COUNTIF($A15:$D15,K$1)</f>
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <f>COUNTIF($A15:$D15,L$1)</f>
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <f>COUNTIF($A15:$D15,M$1)</f>
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <f>COUNTIF($A15:$D15,N$1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>156</v>
+      </c>
+      <c r="B16">
+        <v>3618249.5</v>
+      </c>
+      <c r="C16">
+        <v>24.9</v>
+      </c>
+      <c r="D16" t="s">
+        <v>155</v>
+      </c>
+      <c r="E16">
+        <v>3041886.625</v>
+      </c>
+      <c r="F16">
+        <v>10.6</v>
+      </c>
+      <c r="G16">
+        <v>2610717.1880000001</v>
+      </c>
+      <c r="H16">
+        <v>64.5</v>
+      </c>
+      <c r="I16">
+        <f>COUNTIF($A16:$D16,I$1)</f>
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <f>COUNTIF($A16:$D16,J$1)</f>
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <f>COUNTIF($A16:$D16,K$1)</f>
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <f>COUNTIF($A16:$D16,L$1)</f>
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <f>COUNTIF($A16:$D16,M$1)</f>
+        <v>1</v>
+      </c>
+      <c r="N16">
+        <f>COUNTIF($A16:$D16,N$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>158</v>
+      </c>
+      <c r="B17">
+        <v>3196063.625</v>
+      </c>
+      <c r="C17">
+        <v>13.1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>156</v>
+      </c>
+      <c r="E17">
+        <v>3618249.5</v>
+      </c>
+      <c r="F17">
+        <v>23.3</v>
+      </c>
+      <c r="G17">
+        <v>2648692.375</v>
+      </c>
+      <c r="H17">
+        <v>63.6</v>
+      </c>
+      <c r="I17">
+        <f>COUNTIF($A17:$D17,I$1)</f>
+        <v>1</v>
+      </c>
+      <c r="J17">
+        <f>COUNTIF($A17:$D17,J$1)</f>
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <f>COUNTIF($A17:$D17,K$1)</f>
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <f>COUNTIF($A17:$D17,L$1)</f>
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <f>COUNTIF($A17:$D17,M$1)</f>
+        <v>1</v>
+      </c>
+      <c r="N17">
+        <f>COUNTIF($A17:$D17,N$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>158</v>
+      </c>
+      <c r="B18">
+        <v>3196063.625</v>
+      </c>
+      <c r="C18">
+        <v>21.3</v>
+      </c>
+      <c r="D18" t="s">
+        <v>155</v>
+      </c>
+      <c r="E18">
+        <v>3041886.625</v>
+      </c>
+      <c r="F18">
+        <v>17.3</v>
+      </c>
+      <c r="G18">
+        <v>2375180.0630000001</v>
+      </c>
+      <c r="H18">
+        <v>61.5</v>
+      </c>
+      <c r="I18">
+        <f>COUNTIF($A18:$D18,I$1)</f>
+        <v>1</v>
+      </c>
+      <c r="J18">
+        <f>COUNTIF($A18:$D18,J$1)</f>
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <f>COUNTIF($A18:$D18,K$1)</f>
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <f>COUNTIF($A18:$D18,L$1)</f>
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <f>COUNTIF($A18:$D18,M$1)</f>
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <f>COUNTIF($A18:$D18,N$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>157</v>
+      </c>
+      <c r="B19">
+        <v>2652405.9380000001</v>
+      </c>
+      <c r="C19">
+        <v>12</v>
+      </c>
+      <c r="D19" t="s">
+        <v>158</v>
+      </c>
+      <c r="E19">
+        <v>3196063.625</v>
+      </c>
+      <c r="F19">
+        <v>27</v>
+      </c>
+      <c r="G19">
+        <v>2215579.125</v>
+      </c>
+      <c r="H19">
+        <v>61</v>
+      </c>
+      <c r="I19">
+        <f>COUNTIF($A19:$D19,I$1)</f>
+        <v>1</v>
+      </c>
+      <c r="J19">
+        <f>COUNTIF($A19:$D19,J$1)</f>
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <f>COUNTIF($A19:$D19,K$1)</f>
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <f>COUNTIF($A19:$D19,L$1)</f>
+        <v>1</v>
+      </c>
+      <c r="M19">
+        <f>COUNTIF($A19:$D19,M$1)</f>
+        <v>0</v>
+      </c>
+      <c r="N19">
+        <f>COUNTIF($A19:$D19,N$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>157</v>
+      </c>
+      <c r="B20">
+        <v>2652405.9380000001</v>
+      </c>
+      <c r="C20">
+        <v>14.2</v>
+      </c>
+      <c r="D20" t="s">
+        <v>155</v>
+      </c>
+      <c r="E20">
+        <v>3041886.625</v>
+      </c>
+      <c r="F20">
+        <v>25.2</v>
+      </c>
+      <c r="G20">
+        <v>2147736.4380000001</v>
+      </c>
+      <c r="H20">
+        <v>60.6</v>
+      </c>
+      <c r="I20">
+        <f>COUNTIF($A20:$D20,I$1)</f>
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <f>COUNTIF($A20:$D20,J$1)</f>
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <f>COUNTIF($A20:$D20,K$1)</f>
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <f>COUNTIF($A20:$D20,L$1)</f>
+        <v>1</v>
+      </c>
+      <c r="M20">
+        <f>COUNTIF($A20:$D20,M$1)</f>
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <f>COUNTIF($A20:$D20,N$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>157</v>
+      </c>
+      <c r="B21">
+        <v>2652405.9380000001</v>
+      </c>
+      <c r="C21">
+        <v>2.7</v>
+      </c>
+      <c r="D21" t="s">
+        <v>152</v>
+      </c>
+      <c r="E21">
+        <v>4143004.3130000001</v>
+      </c>
+      <c r="F21">
+        <v>37.700000000000003</v>
+      </c>
+      <c r="G21">
+        <v>2537372.125</v>
+      </c>
+      <c r="H21">
+        <v>59.6</v>
+      </c>
+      <c r="I21">
+        <f>COUNTIF($A21:$D21,I$1)</f>
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <f>COUNTIF($A21:$D21,J$1)</f>
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <f>COUNTIF($A21:$D21,K$1)</f>
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <f>COUNTIF($A21:$D21,L$1)</f>
+        <v>1</v>
+      </c>
+      <c r="M21">
+        <f>COUNTIF($A21:$D21,M$1)</f>
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <f>COUNTIF($A21:$D21,N$1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>157</v>
+      </c>
+      <c r="B22">
+        <v>2652405.9380000001</v>
+      </c>
+      <c r="C22">
+        <v>8.4</v>
+      </c>
+      <c r="D22" t="s">
+        <v>156</v>
+      </c>
+      <c r="E22">
+        <v>3618249.5</v>
+      </c>
+      <c r="F22">
+        <v>32.9</v>
+      </c>
+      <c r="G22">
+        <v>2319196.1880000001</v>
+      </c>
+      <c r="H22">
+        <v>58.7</v>
+      </c>
+      <c r="I22">
+        <f>COUNTIF($A22:$D22,I$1)</f>
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <f>COUNTIF($A22:$D22,J$1)</f>
+        <v>0</v>
+      </c>
+      <c r="K22">
+        <f>COUNTIF($A22:$D22,K$1)</f>
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <f>COUNTIF($A22:$D22,L$1)</f>
+        <v>1</v>
+      </c>
+      <c r="M22">
+        <f>COUNTIF($A22:$D22,M$1)</f>
+        <v>1</v>
+      </c>
+      <c r="N22">
+        <f>COUNTIF($A22:$D22,N$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>154</v>
+      </c>
+      <c r="B23">
+        <v>3294591.8130000001</v>
+      </c>
+      <c r="C23">
+        <v>53.5</v>
+      </c>
+      <c r="D23" t="s">
+        <v>159</v>
+      </c>
+      <c r="E23">
+        <v>1603712.75</v>
+      </c>
+      <c r="F23">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="G23">
+        <v>1452565</v>
+      </c>
+      <c r="H23">
+        <v>42.2</v>
+      </c>
+      <c r="I23">
+        <f>COUNTIF($A23:$D23,I$1)</f>
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <f>COUNTIF($A23:$D23,J$1)</f>
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <f>COUNTIF($A23:$D23,K$1)</f>
+        <v>1</v>
+      </c>
+      <c r="L23">
+        <f>COUNTIF($A23:$D23,L$1)</f>
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <f>COUNTIF($A23:$D23,M$1)</f>
+        <v>0</v>
+      </c>
+      <c r="N23">
+        <f>COUNTIF($A23:$D23,N$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>159</v>
+      </c>
+      <c r="B24">
+        <v>1603712.75</v>
+      </c>
+      <c r="C24">
+        <v>7.6</v>
+      </c>
+      <c r="D24" t="s">
+        <v>155</v>
+      </c>
+      <c r="E24">
+        <v>3041886.625</v>
+      </c>
+      <c r="F24">
+        <v>51.3</v>
+      </c>
+      <c r="G24">
+        <v>1353150.5630000001</v>
+      </c>
+      <c r="H24">
+        <v>41.1</v>
+      </c>
+      <c r="I24">
+        <f>COUNTIF($A24:$D24,I$1)</f>
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <f>COUNTIF($A24:$D24,J$1)</f>
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <f>COUNTIF($A24:$D24,K$1)</f>
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <f>COUNTIF($A24:$D24,L$1)</f>
+        <v>0</v>
+      </c>
+      <c r="M24">
+        <f>COUNTIF($A24:$D24,M$1)</f>
+        <v>0</v>
+      </c>
+      <c r="N24">
+        <f>COUNTIF($A24:$D24,N$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>153</v>
+      </c>
+      <c r="B25">
+        <v>3798352.5630000001</v>
+      </c>
+      <c r="C25">
+        <v>58.9</v>
+      </c>
+      <c r="D25" t="s">
+        <v>159</v>
+      </c>
+      <c r="E25">
+        <v>1603712.75</v>
+      </c>
+      <c r="F25">
+        <v>2.6</v>
+      </c>
+      <c r="G25">
+        <v>1500397.5630000001</v>
+      </c>
+      <c r="H25">
+        <v>38.5</v>
+      </c>
+      <c r="I25">
+        <f>COUNTIF($A25:$D25,I$1)</f>
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <f>COUNTIF($A25:$D25,J$1)</f>
+        <v>1</v>
+      </c>
+      <c r="K25">
+        <f>COUNTIF($A25:$D25,K$1)</f>
+        <v>0</v>
+      </c>
+      <c r="L25">
+        <f>COUNTIF($A25:$D25,L$1)</f>
+        <v>0</v>
+      </c>
+      <c r="M25">
+        <f>COUNTIF($A25:$D25,M$1)</f>
+        <v>0</v>
+      </c>
+      <c r="N25">
+        <f>COUNTIF($A25:$D25,N$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>157</v>
+      </c>
+      <c r="B26">
+        <v>2652405.9380000001</v>
+      </c>
+      <c r="C26">
+        <v>47.9</v>
+      </c>
+      <c r="D26" t="s">
+        <v>159</v>
+      </c>
+      <c r="E26">
+        <v>1603712.75</v>
+      </c>
+      <c r="F26">
+        <v>13.8</v>
+      </c>
+      <c r="G26">
+        <v>1180473.3130000001</v>
+      </c>
+      <c r="H26">
+        <v>38.4</v>
+      </c>
+      <c r="I26">
+        <f>COUNTIF($A26:$D26,I$1)</f>
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <f>COUNTIF($A26:$D26,J$1)</f>
+        <v>0</v>
+      </c>
+      <c r="K26">
+        <f>COUNTIF($A26:$D26,K$1)</f>
+        <v>0</v>
+      </c>
+      <c r="L26">
+        <f>COUNTIF($A26:$D26,L$1)</f>
+        <v>1</v>
+      </c>
+      <c r="M26">
+        <f>COUNTIF($A26:$D26,M$1)</f>
+        <v>0</v>
+      </c>
+      <c r="N26">
+        <f>COUNTIF($A26:$D26,N$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>158</v>
+      </c>
+      <c r="B27">
+        <v>3196063.625</v>
+      </c>
+      <c r="C27">
+        <v>54.5</v>
+      </c>
+      <c r="D27" t="s">
+        <v>159</v>
+      </c>
+      <c r="E27">
+        <v>1603712.75</v>
+      </c>
+      <c r="F27">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="G27">
+        <v>1276347.5630000001</v>
+      </c>
+      <c r="H27">
+        <v>36.200000000000003</v>
+      </c>
+      <c r="I27">
+        <f>COUNTIF($A27:$D27,I$1)</f>
+        <v>1</v>
+      </c>
+      <c r="J27">
+        <f>COUNTIF($A27:$D27,J$1)</f>
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <f>COUNTIF($A27:$D27,K$1)</f>
+        <v>0</v>
+      </c>
+      <c r="L27">
+        <f>COUNTIF($A27:$D27,L$1)</f>
+        <v>0</v>
+      </c>
+      <c r="M27">
+        <f>COUNTIF($A27:$D27,M$1)</f>
+        <v>0</v>
+      </c>
+      <c r="N27">
+        <f>COUNTIF($A27:$D27,N$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>152</v>
+      </c>
+      <c r="B28">
+        <v>4143004.3130000001</v>
+      </c>
+      <c r="C28">
+        <v>62.1</v>
+      </c>
+      <c r="D28" t="s">
+        <v>159</v>
+      </c>
+      <c r="E28">
+        <v>1603712.75</v>
+      </c>
+      <c r="F28">
+        <v>2.1</v>
+      </c>
+      <c r="G28">
+        <v>1515895</v>
+      </c>
+      <c r="H28">
+        <v>35.799999999999997</v>
+      </c>
+      <c r="I28">
+        <f>COUNTIF($A28:$D28,I$1)</f>
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <f>COUNTIF($A28:$D28,J$1)</f>
+        <v>0</v>
+      </c>
+      <c r="K28">
+        <f>COUNTIF($A28:$D28,K$1)</f>
+        <v>0</v>
+      </c>
+      <c r="L28">
+        <f>COUNTIF($A28:$D28,L$1)</f>
+        <v>0</v>
+      </c>
+      <c r="M28">
+        <f>COUNTIF($A28:$D28,M$1)</f>
+        <v>0</v>
+      </c>
+      <c r="N28">
+        <f>COUNTIF($A28:$D28,N$1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>159</v>
+      </c>
+      <c r="B29">
+        <v>1603712.75</v>
+      </c>
+      <c r="C29">
+        <v>6.1</v>
+      </c>
+      <c r="D29" t="s">
+        <v>156</v>
+      </c>
+      <c r="E29">
+        <v>3618249.5</v>
+      </c>
+      <c r="F29">
+        <v>58.4</v>
+      </c>
+      <c r="G29">
+        <v>1369402.0630000001</v>
+      </c>
+      <c r="H29">
+        <v>35.5</v>
+      </c>
+      <c r="I29">
+        <f>COUNTIF($A29:$D29,I$1)</f>
+        <v>0</v>
+      </c>
+      <c r="J29">
+        <f>COUNTIF($A29:$D29,J$1)</f>
+        <v>0</v>
+      </c>
+      <c r="K29">
+        <f>COUNTIF($A29:$D29,K$1)</f>
+        <v>0</v>
+      </c>
+      <c r="L29">
+        <f>COUNTIF($A29:$D29,L$1)</f>
+        <v>0</v>
+      </c>
+      <c r="M29">
+        <f>COUNTIF($A29:$D29,M$1)</f>
+        <v>1</v>
+      </c>
+      <c r="N29">
+        <f>COUNTIF($A29:$D29,N$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="I2:N29">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AF8DCEA-4EAB-49C3-B3B5-D46D386FC311}">
   <dimension ref="A1:R37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R35" sqref="R35"/>
+      <selection activeCell="R34" sqref="R34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4093,7 +5600,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D30C308-BE0C-477B-845E-425B7496B215}">
   <dimension ref="A1:P18"/>
   <sheetViews>
@@ -4608,7 +6115,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{971B3941-39EB-43BC-8C0B-5F8722A04C12}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -4660,11 +6167,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99AAD824-D627-40E0-BEE4-ABF7B5BBAA55}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>

</xml_diff>